<commit_message>
add sheet and col diff on excel differ
</commit_message>
<xml_diff>
--- a/test/table_differ/excel_differ/dest/2.xlsx
+++ b/test/table_differ/excel_differ/dest/2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\Python\gameff-toolset\test\table_differ\excel_differ\dst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\Python\gameff-toolset\test\table_differ\excel_differ\dest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FF1AFF-E3DE-43BA-8B64-19EB98A7DE4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612FEABB-A2C7-4EC7-B149-F7D14380359C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,31 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nama</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kaka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -346,12 +371,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -360,6 +411,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA58EA6-3352-45E0-B4E6-7D964F278460}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E233C28A-57F0-43D9-B084-DF76822A5C80}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -369,17 +441,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E233C28A-57F0-43D9-B084-DF76822A5C80}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>